<commit_message>
Nuevo sube(3).dia + agrego casos de usos
</commit_message>
<xml_diff>
--- a/Proyecto Sube/Documentación/Diseño/Casos de usos/Casos de uso SUBE.xlsx
+++ b/Proyecto Sube/Documentación/Diseño/Casos de usos/Casos de uso SUBE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Objetos2\Proyecto Sube\Documentación\Diseño\Casos de usos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA8A454-883C-490B-AA6B-D3E288EC75C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506553FD-12B0-4A0B-8405-0B5C43671B9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="270" yWindow="600" windowWidth="28215" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
   <si>
     <t>Nro.de Caso</t>
   </si>
@@ -215,13 +215,37 @@
   </si>
   <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>Devuelve si la tarjeta tiene o no la tarifa social</t>
+  </si>
+  <si>
+    <t>tieneSaldoNegativo</t>
+  </si>
+  <si>
+    <t>devuelve true o false si tiene saldo negativo</t>
+  </si>
+  <si>
+    <t>cargaMinima</t>
+  </si>
+  <si>
+    <t>devuelve el monto minimo que debe pagar para cargar la sube</t>
+  </si>
+  <si>
+    <t>cerroViajeTren</t>
+  </si>
+  <si>
+    <t>devuelve true o false si cerro el ultimo viaje en tren que hizo</t>
+  </si>
+  <si>
+    <t>tieneTarifaSocial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -230,6 +254,12 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -252,9 +282,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,9 +629,7 @@
   </sheetPr>
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -612,7 +641,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1003,15 +1032,69 @@
       <c r="A21" s="1">
         <v>20</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
@@ -1069,5 +1152,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualización casos de uso
Se eliminaron los casos de uso de las clases Tren, Colectivo y Subte
</commit_message>
<xml_diff>
--- a/Proyecto Sube/Documentación/Diseño/Casos de usos/Casos de uso SUBE.xlsx
+++ b/Proyecto Sube/Documentación/Diseño/Casos de usos/Casos de uso SUBE.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Objetos2\Proyecto Sube\Documentación\Diseño\Casos de usos\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506553FD-12B0-4A0B-8405-0B5C43671B9C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="270" yWindow="600" windowWidth="28215" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="270" yWindow="600" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="64">
   <si>
     <t>Nro.de Caso</t>
   </si>
@@ -94,15 +88,6 @@
     <t>agregarMovimiento</t>
   </si>
   <si>
-    <t>Tren</t>
-  </si>
-  <si>
-    <t>Colectivo</t>
-  </si>
-  <si>
-    <t>Subte</t>
-  </si>
-  <si>
     <t>Realizar la carga de saldo a una tarjeta.</t>
   </si>
   <si>
@@ -185,24 +170,6 @@
   </si>
   <si>
     <t>Trae una tarjeta por el usuario asignado.</t>
-  </si>
-  <si>
-    <t>Procesa el precio según sube o baja (y donde baja).</t>
-  </si>
-  <si>
-    <t>Procesa el precio según el precio indicado por el chofer.</t>
-  </si>
-  <si>
-    <t>Procesa el precio único del subte.</t>
-  </si>
-  <si>
-    <t>float: precio; boolean: asciende = true;</t>
-  </si>
-  <si>
-    <t>float: precio = null; boolean: asciende;</t>
-  </si>
-  <si>
-    <t>float: precio = null ; boolean: asciende = true;</t>
   </si>
   <si>
     <t>aplicarRedSube</t>
@@ -244,7 +211,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -346,7 +313,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,26 +346,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,23 +381,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -623,13 +556,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -671,13 +606,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -691,13 +626,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -711,10 +646,10 @@
         <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -728,10 +663,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -745,10 +680,10 @@
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -762,10 +697,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>6</v>
@@ -782,10 +717,10 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
@@ -802,10 +737,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>6</v>
@@ -822,13 +757,13 @@
         <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -842,13 +777,13 @@
         <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -862,10 +797,10 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -879,13 +814,13 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -899,10 +834,10 @@
         <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>14</v>
@@ -919,10 +854,10 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>14</v>
@@ -939,13 +874,13 @@
         <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -953,19 +888,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -973,19 +908,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -993,19 +925,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1013,19 +942,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1033,68 +959,26 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="A22" s="1"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="A23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
@@ -1135,20 +1019,11 @@
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>